<commit_message>
aktualizace oponentury 3. iterace ŠIP
</commit_message>
<xml_diff>
--- a/oponentura ŠIP/3. iterace.xlsx
+++ b/oponentura ŠIP/3. iterace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Oponentura (checklist) k ŠIP - 1. iterace</t>
   </si>
@@ -52,9 +52,6 @@
     <t>BPM</t>
   </si>
   <si>
-    <t>BDM</t>
-  </si>
-  <si>
     <t>Use Case</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
   </si>
   <si>
     <t>Zápočet</t>
-  </si>
-  <si>
-    <t>chybí zápočet</t>
   </si>
   <si>
     <t>více</t>
@@ -567,11 +561,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,110 +620,110 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -737,59 +731,48 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>